<commit_message>
example - add arrageOption example
</commit_message>
<xml_diff>
--- a/example/excel/example1_grocery_stock.xlsx
+++ b/example/excel/example1_grocery_stock.xlsx
@@ -102,7 +102,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:C4"/>
+  <dimension ref="A1:D3"/>
   <sheetViews>
     <sheetView workbookViewId="0" tabSelected="true"/>
   </sheetViews>
@@ -113,42 +113,40 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="C1" t="s">
-        <v>8</v>
+        <v>2</v>
+      </c>
+      <c r="D1" t="s">
+        <v>3</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="B2" t="s">
         <v>5</v>
       </c>
       <c r="C2" t="s">
-        <v>9</v>
+        <v>6</v>
+      </c>
+      <c r="D2" t="s">
+        <v>7</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s">
-        <v>2</v>
+        <v>8</v>
       </c>
       <c r="B3" t="s">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="C3" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="4">
-      <c r="A4" t="s">
-        <v>3</v>
-      </c>
-      <c r="B4" t="s">
-        <v>7</v>
-      </c>
-      <c r="C4" t="s">
+      <c r="D3" t="s">
         <v>11</v>
       </c>
     </row>
@@ -159,7 +157,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:D3"/>
+  <dimension ref="A1:C4"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -170,40 +168,42 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>12</v>
+        <v>4</v>
       </c>
       <c r="C1" t="s">
-        <v>13</v>
-      </c>
-      <c r="D1" t="s">
-        <v>14</v>
+        <v>8</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s">
-        <v>4</v>
+        <v>12</v>
       </c>
       <c r="B2" t="s">
         <v>5</v>
       </c>
       <c r="C2" t="s">
-        <v>6</v>
-      </c>
-      <c r="D2" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s">
-        <v>8</v>
+        <v>13</v>
       </c>
       <c r="B3" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="C3" t="s">
         <v>10</v>
       </c>
-      <c r="D3" t="s">
+    </row>
+    <row r="4">
+      <c r="A4" t="s">
+        <v>14</v>
+      </c>
+      <c r="B4" t="s">
+        <v>7</v>
+      </c>
+      <c r="C4" t="s">
         <v>11</v>
       </c>
     </row>

</xml_diff>